<commit_message>
modified lesson 9 and 10
</commit_message>
<xml_diff>
--- a/lesson10/report.xlsx
+++ b/lesson10/report.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\PEO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\PEO\lesson10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BFD5AD-29BC-40AC-A6CB-75910CCB2276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0423E7B-B69F-4BFB-B2F3-310B513E0D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -404,13 +405,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -438,7 +439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -461,16 +462,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5618FB2-EED2-4E8C-AB12-DFFB78093E39}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -484,7 +485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -495,7 +496,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -506,7 +507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -517,7 +518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -528,7 +529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -539,7 +540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -550,7 +551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -561,7 +562,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -585,12 +586,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -615,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -626,7 +627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -640,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -654,4 +655,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9F9AF3-899E-4291-B830-6BB7533F276E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>